<commit_message>
Added some function comments
</commit_message>
<xml_diff>
--- a/CAR - Accessibility Review Template.xlsx
+++ b/CAR - Accessibility Review Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="11775"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="11775" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Accessibility Review" sheetId="2" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="DD Menu" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1" hidden="1">Charts!$B$4:$C$12</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity" hidden="1">Charts!$B$4:$C$12</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
     <definedName name="category">'DD Menu'!$E$4:$G$4</definedName>
     <definedName name="Checklist">Checklist!$B$3:$C$14</definedName>
     <definedName name="Color">'Error &amp; Descriptions'!$D$6:$D$8</definedName>
@@ -53,7 +53,6 @@
     <definedName name="YesOrNo">'DD Menu'!$K$4:$K$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -93,7 +92,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issue_Severity">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -102,7 +101,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -111,7 +110,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues Location" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -2421,12 +2420,7 @@
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="39000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -4248,7 +4242,7 @@
   </sheetPr>
   <dimension ref="B1:L155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -6526,8 +6520,8 @@
   </sheetPr>
   <dimension ref="B2:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27:S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated EXE files and the excel template to have warnings about what it doesn't check
</commit_message>
<xml_diff>
--- a/CAR - Accessibility Review Template.xlsx
+++ b/CAR - Accessibility Review Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="11775" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="11775"/>
   </bookViews>
   <sheets>
     <sheet name="Accessibility Review" sheetId="2" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="DD Menu" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity" hidden="1">Charts!$B$4:$C$12</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1" hidden="1">Charts!$B$4:$C$12</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
     <definedName name="category">'DD Menu'!$E$4:$G$4</definedName>
     <definedName name="Checklist">Checklist!$B$3:$C$14</definedName>
     <definedName name="Color">'Error &amp; Descriptions'!$D$6:$D$8</definedName>
@@ -92,7 +92,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issue_Severity">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -101,7 +101,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -110,7 +110,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues Location" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1859,6 +1859,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFFD505"/>
       <color rgb="FFFF4747"/>
       <color rgb="FFFF2525"/>
       <color rgb="FFFF4F4F"/>
@@ -1867,7 +1868,6 @@
       <color rgb="FF00D661"/>
       <color rgb="FFBC0000"/>
       <color rgb="FFFF6161"/>
-      <color rgb="FFFFD505"/>
       <color rgb="FF91CE4E"/>
     </mruColors>
   </colors>
@@ -3352,14 +3352,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
@@ -3370,7 +3370,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11601450" y="9458324"/>
+          <a:off x="11601450" y="11477624"/>
           <a:ext cx="4095750" cy="8486776"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3444,9 +3444,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>457202</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3456,9 +3456,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="11582400" y="3467098"/>
-          <a:ext cx="4143375" cy="5667377"/>
-          <a:chOff x="12668250" y="3733798"/>
-          <a:chExt cx="2423774" cy="5667377"/>
+          <a:ext cx="4143377" cy="7772402"/>
+          <a:chOff x="12668249" y="3733798"/>
+          <a:chExt cx="2423775" cy="7772402"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -3695,7 +3695,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="12668250" y="8258175"/>
+            <a:off x="12668249" y="10363200"/>
             <a:ext cx="2419350" cy="1143000"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -3823,6 +3823,114 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>459163</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11591925" y="8000999"/>
+          <a:ext cx="4135813" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFD505"/>
+        </a:solidFill>
+        <a:ln w="19050" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The report generator does not check Quizzes</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> or Assignments</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="628650" lvl="1" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>These will have to be manually checked</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> along with fixing the issues found</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" lvl="0" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If you used this program to check a directory of files this of course does not check any content that is online (in Buzz</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> this would mean and Rich Text Content / Quizzes / Assessments)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" lvl="0" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>This does not check color.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4242,8 +4350,8 @@
   </sheetPr>
   <dimension ref="B1:L155"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6520,7 +6628,7 @@
   </sheetPr>
   <dimension ref="B2:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="S27" sqref="S27:S28"/>
     </sheetView>
   </sheetViews>
@@ -6665,8 +6773,8 @@
   </sheetPr>
   <dimension ref="B1:S28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="K1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6:P10"/>
+    <sheetView showGridLines="0" topLeftCell="B2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7566,8 +7674,8 @@
     <col min="9" max="9" width="21.5703125" style="2" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" style="2" customWidth="1"/>
     <col min="11" max="26" width="30.7109375" style="2" customWidth="1"/>
-    <col min="27" max="27" width="11.140625" style="2" customWidth="1"/>
-    <col min="28" max="16384" width="11.140625" style="2"/>
+    <col min="27" max="28" width="11.140625" style="2" customWidth="1"/>
+    <col min="29" max="16384" width="11.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Will now search through Quizzes and Assignments
</commit_message>
<xml_diff>
--- a/CAR - Accessibility Review Template.xlsx
+++ b/CAR - Accessibility Review Template.xlsx
@@ -19,9 +19,9 @@
     <sheet name="DD Menu" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1" hidden="1">Charts!$B$4:$C$12</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity" hidden="1">Charts!$B$4:$C$12</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
     <definedName name="category">'DD Menu'!$E$4:$G$4</definedName>
     <definedName name="Checklist">Checklist!$B$3:$C$14</definedName>
     <definedName name="Color">'Error &amp; Descriptions'!$D$6:$D$8</definedName>
@@ -92,7 +92,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issue_Severity">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -101,7 +101,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -110,7 +110,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues Location" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1926,7 +1926,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2314,9 +2313,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2417,7 +2414,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3929,6 +3925,33 @@
             <a:t>This does not check color.</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:pPr marL="171450" lvl="0" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>This report is not perfect and is to be used as a guide</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="628650" lvl="1" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Some items may not need to be changed, as well as some items that should be changed may not be found</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" lvl="0" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>

</xml_diff>

<commit_message>
Added check for video tags
</commit_message>
<xml_diff>
--- a/CAR - Accessibility Review Template.xlsx
+++ b/CAR - Accessibility Review Template.xlsx
@@ -19,9 +19,9 @@
     <sheet name="DD Menu" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity" hidden="1">Charts!$B$4:$C$12</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1" hidden="1">Charts!$B$4:$C$12</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
     <definedName name="category">'DD Menu'!$E$4:$G$4</definedName>
     <definedName name="Checklist">Checklist!$B$3:$C$14</definedName>
     <definedName name="Color">'Error &amp; Descriptions'!$D$6:$D$8</definedName>
@@ -92,7 +92,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issue_Severity">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -101,7 +101,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -110,7 +110,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues Location" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1926,6 +1926,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2313,7 +2314,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2414,6 +2417,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3874,34 +3878,6 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="171450" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>The report generator does not check Quizzes</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> or Assignments</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="628650" lvl="1" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>These will have to be manually checked</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> along with fixing the issues found</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
           <a:pPr marL="171450" lvl="0" indent="-171450">
             <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             <a:buChar char="•"/>
@@ -3950,7 +3926,10 @@
             <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             <a:buChar char="•"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>The report can only check quizzes if your account has the correct authorization</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4373,8 +4352,8 @@
   </sheetPr>
   <dimension ref="B1:L155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added another accessibility issue that needed to be converted correctly to template
</commit_message>
<xml_diff>
--- a/CAR - Accessibility Review Template.xlsx
+++ b/CAR - Accessibility Review Template.xlsx
@@ -19,9 +19,9 @@
     <sheet name="DD Menu" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1" hidden="1">Charts!$B$4:$C$12</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity" hidden="1">Charts!$B$4:$C$12</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
     <definedName name="category">'DD Menu'!$E$4:$G$4</definedName>
     <definedName name="Checklist">Checklist!$B$3:$C$14</definedName>
     <definedName name="Color">'Error &amp; Descriptions'!$D$6:$D$8</definedName>
@@ -92,7 +92,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issue_Severity">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -101,7 +101,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -110,7 +110,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues Location" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1926,7 +1926,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2314,9 +2313,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2417,7 +2414,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3928,7 +3924,17 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>The report can only check quizzes if your account has the correct authorization</a:t>
+            <a:t>The program can only check quizzes if your account has the correct authorization</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" lvl="0" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>The program can not check if rubric tables are accessible</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4352,7 +4358,7 @@
   </sheetPr>
   <dimension ref="B1:L155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Touched up the template
</commit_message>
<xml_diff>
--- a/CAR - Accessibility Review Template.xlsx
+++ b/CAR - Accessibility Review Template.xlsx
@@ -19,9 +19,9 @@
     <sheet name="DD Menu" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1" hidden="1">Charts!$B$4:$C$12</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity" hidden="1">Charts!$B$4:$C$12</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues" hidden="1">'Accessibility Review'!$B$9:$J$142</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation" hidden="1">'Accessibility Review'!$C$9:$C$142</definedName>
     <definedName name="category">'DD Menu'!$E$4:$G$4</definedName>
     <definedName name="Checklist">Checklist!$B$3:$C$14</definedName>
     <definedName name="Color">'Error &amp; Descriptions'!$D$6:$D$8</definedName>
@@ -92,7 +92,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issue_Severity">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssue_Severity"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -101,7 +101,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssues"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -110,7 +110,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Issues Location" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TESTAccessibilityReviewTemplate.xlsxIssuesLocation"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1315,9 +1315,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1396,6 +1393,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1926,7 +1926,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2314,9 +2313,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2417,7 +2414,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3126,14 +3122,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>189297</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>371475</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>532202</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>64413</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>476250</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3143,7 +3139,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="11581197" y="190500"/>
-          <a:ext cx="4219580" cy="3207663"/>
+          <a:ext cx="4219580" cy="2362200"/>
           <a:chOff x="10086057" y="-16668"/>
           <a:chExt cx="3886226" cy="3714407"/>
         </a:xfrm>
@@ -3173,8 +3169,8 @@
           </a:xfrm>
           <a:grpFill/>
         </xdr:grpSpPr>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-          <mc:Choice Requires="sle15">
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
             <xdr:graphicFrame macro="">
               <xdr:nvGraphicFramePr>
                 <xdr:cNvPr id="3" name="Issue Type"/>
@@ -3191,7 +3187,7 @@
               </a:graphic>
             </xdr:graphicFrame>
           </mc:Choice>
-          <mc:Fallback xmlns="">
+          <mc:Fallback>
             <xdr:sp macro="" textlink="">
               <xdr:nvSpPr>
                 <xdr:cNvPr id="0" name=""/>
@@ -3201,8 +3197,8 @@
               </xdr:nvSpPr>
               <xdr:spPr>
                 <a:xfrm>
-                  <a:off x="13616031" y="378758"/>
-                  <a:ext cx="2184746" cy="3202642"/>
+                  <a:off x="13616031" y="195847"/>
+                  <a:ext cx="2184746" cy="2351520"/>
                 </a:xfrm>
                 <a:prstGeom prst="rect">
                   <a:avLst/>
@@ -3230,8 +3226,8 @@
             </xdr:sp>
           </mc:Fallback>
         </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-          <mc:Choice Requires="sle15">
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
             <xdr:graphicFrame macro="">
               <xdr:nvGraphicFramePr>
                 <xdr:cNvPr id="4" name="Severity"/>
@@ -3248,7 +3244,7 @@
               </a:graphic>
             </xdr:graphicFrame>
           </mc:Choice>
-          <mc:Fallback xmlns="">
+          <mc:Fallback>
             <xdr:sp macro="" textlink="">
               <xdr:nvSpPr>
                 <xdr:cNvPr id="0" name=""/>
@@ -3258,8 +3254,8 @@
               </xdr:nvSpPr>
               <xdr:spPr>
                 <a:xfrm>
-                  <a:off x="11590726" y="371475"/>
-                  <a:ext cx="1990555" cy="1591348"/>
+                  <a:off x="11590726" y="190500"/>
+                  <a:ext cx="1990555" cy="1168437"/>
                 </a:xfrm>
                 <a:prstGeom prst="rect">
                   <a:avLst/>
@@ -3288,8 +3284,8 @@
           </mc:Fallback>
         </mc:AlternateContent>
       </xdr:grpSp>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-        <mc:Choice Requires="sle15">
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
           <xdr:graphicFrame macro="">
             <xdr:nvGraphicFramePr>
               <xdr:cNvPr id="8" name="Completion"/>
@@ -3306,7 +3302,7 @@
             </a:graphic>
           </xdr:graphicFrame>
         </mc:Choice>
-        <mc:Fallback xmlns="">
+        <mc:Fallback>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
               <xdr:cNvPr id="0" name=""/>
@@ -3316,8 +3312,8 @@
             </xdr:nvSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="11581197" y="2005271"/>
-                <a:ext cx="1991931" cy="1583392"/>
+                <a:off x="11581197" y="1390104"/>
+                <a:ext cx="1991931" cy="1162596"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
                 <a:avLst/>
@@ -3351,116 +3347,101 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57148</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:colOff>506787</xdr:colOff>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="" fLocksText="0">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="TextBox 9" title="Review Overview"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11601450" y="11725274"/>
-          <a:ext cx="4095750" cy="8486776"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln/>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="0"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="548640" tIns="182880" rIns="274320" bIns="182880" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1"/>
-            <a:t>Overview Notes:</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400" b="0"/>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>
-            </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData fPrintsWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>133348</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>466727</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="12" name="Group 11"/>
+        <xdr:cNvPr id="2" name="Group 1"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11591925" y="3848098"/>
-          <a:ext cx="4143377" cy="7772402"/>
-          <a:chOff x="12668249" y="3733798"/>
-          <a:chExt cx="2423775" cy="7772402"/>
+          <a:off x="11639549" y="2628898"/>
+          <a:ext cx="4135813" cy="16630652"/>
+          <a:chOff x="11639549" y="2628898"/>
+          <a:chExt cx="4135813" cy="16630652"/>
         </a:xfrm>
       </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="" fLocksText="0">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="TextBox 9" title="Review Overview"/>
+          <xdr:cNvSpPr txBox="1">
+            <a:spLocks/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11659580" y="10772774"/>
+            <a:ext cx="4095750" cy="8486776"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln/>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="548640" tIns="182880" rIns="274320" bIns="182880" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
+              <a:t>Overview Notes:</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr lvl="0"/>
+            <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr lvl="0"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+              <a:t>
+            </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
           <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -3468,8 +3449,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="12668250" y="3733798"/>
-            <a:ext cx="2419350" cy="3343276"/>
+            <a:off x="11639549" y="2628898"/>
+            <a:ext cx="4135812" cy="3343276"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3615,8 +3596,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="12672674" y="7191375"/>
-            <a:ext cx="2419350" cy="952500"/>
+            <a:off x="11639549" y="6057900"/>
+            <a:ext cx="4135812" cy="952500"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3695,8 +3676,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="12668249" y="10363200"/>
-            <a:ext cx="2419350" cy="1143000"/>
+            <a:off x="11639549" y="9553575"/>
+            <a:ext cx="4135812" cy="1143000"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3822,141 +3803,126 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="TextBox 13"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11639549" y="7077074"/>
+            <a:ext cx="4135813" cy="2419351"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFD505"/>
+          </a:solidFill>
+          <a:ln w="19050" cmpd="sng">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="171450" lvl="0" indent="-171450">
+              <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:buChar char="•"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>If you used this program to check a directory of files this of course does not check any content that is online (in Buzz</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> this would mean and Rich Text Content / Quizzes / Assessments)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="171450" lvl="0" indent="-171450">
+              <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:buChar char="•"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t>This does not check color.</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="171450" lvl="0" indent="-171450">
+              <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:buChar char="•"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t>This report is not perfect and is to be used as a guide</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="628650" lvl="1" indent="-171450">
+              <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:buChar char="•"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t>Some items may not need to be changed, as well as some items that should be changed may not be found</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="171450" lvl="0" indent="-171450">
+              <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:buChar char="•"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t>The program can only check quizzes if your account has the correct authorization</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="171450" lvl="0" indent="-171450">
+              <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:buChar char="•"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t>The program can not check if rubric tables are accessibl</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+              <a:t>e</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="171450" lvl="0" indent="-171450">
+              <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:buChar char="•"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+              <a:t>The program also cannot tell if a Language course is using the correct language tags for screen readers</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
     </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>468688</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="TextBox 13"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11601450" y="7934324"/>
-          <a:ext cx="4135813" cy="2419351"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFD505"/>
-        </a:solidFill>
-        <a:ln w="19050" cmpd="sng">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="171450" lvl="0" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>If you used this program to check a directory of files this of course does not check any content that is online (in Buzz</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> this would mean and Rich Text Content / Quizzes / Assessments)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="171450" lvl="0" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>This does not check color.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="171450" lvl="0" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>This report is not perfect and is to be used as a guide</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="628650" lvl="1" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Some items may not need to be changed, as well as some items that should be changed may not be found</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="171450" lvl="0" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>The program can only check quizzes if your account has the correct authorization</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="171450" lvl="0" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>The program can not check if rubric tables are accessibl</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>e</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="171450" lvl="0" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>The program also cannot tell if a Language course is using the correct language tags for screen readers</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4377,7 +4343,7 @@
   <dimension ref="B1:L155"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4387,7 +4353,7 @@
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="39.140625" style="44" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="43" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
@@ -4432,7 +4398,7 @@
       <c r="J3" s="80"/>
     </row>
     <row r="4" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="64" t="s">
         <v>89</v>
       </c>
       <c r="C4" s="77"/>
@@ -4465,10 +4431,10 @@
       <c r="D6" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="45"/>
+      <c r="F6" s="44"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -4497,10 +4463,10 @@
       <c r="D8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="45" t="s">
         <v>97</v>
       </c>
       <c r="G8" s="16" t="s">
@@ -4525,7 +4491,7 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="50">
+      <c r="J9" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4540,7 +4506,7 @@
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="50">
+      <c r="J10" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4555,7 +4521,7 @@
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
-      <c r="J11" s="50">
+      <c r="J11" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4570,7 +4536,7 @@
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
-      <c r="J12" s="50">
+      <c r="J12" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4585,7 +4551,7 @@
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
-      <c r="J13" s="50">
+      <c r="J13" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4601,7 +4567,7 @@
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
-      <c r="J14" s="50">
+      <c r="J14" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4617,7 +4583,7 @@
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
-      <c r="J15" s="50">
+      <c r="J15" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4633,7 +4599,7 @@
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
-      <c r="J16" s="50">
+      <c r="J16" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4649,7 +4615,7 @@
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
-      <c r="J17" s="50">
+      <c r="J17" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4665,7 +4631,7 @@
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
-      <c r="J18" s="50">
+      <c r="J18" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4681,7 +4647,7 @@
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
-      <c r="J19" s="50">
+      <c r="J19" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4697,7 +4663,7 @@
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
-      <c r="J20" s="50">
+      <c r="J20" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4713,7 +4679,7 @@
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
-      <c r="J21" s="50">
+      <c r="J21" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4728,7 +4694,7 @@
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
-      <c r="J22" s="50">
+      <c r="J22" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4743,7 +4709,7 @@
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
-      <c r="J23" s="50">
+      <c r="J23" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4758,7 +4724,7 @@
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
-      <c r="J24" s="50">
+      <c r="J24" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4773,7 +4739,7 @@
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
-      <c r="J25" s="50">
+      <c r="J25" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4788,7 +4754,7 @@
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
-      <c r="J26" s="50">
+      <c r="J26" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4803,7 +4769,7 @@
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
-      <c r="J27" s="50">
+      <c r="J27" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4818,7 +4784,7 @@
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
-      <c r="J28" s="50">
+      <c r="J28" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
@@ -4833,1735 +4799,1735 @@
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
-      <c r="J29" s="50">
+      <c r="J29" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
-      <c r="C30" s="58"/>
+      <c r="C30" s="57"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
-      <c r="J30" s="50">
+      <c r="J30" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" s="17"/>
-      <c r="C31" s="58"/>
+      <c r="C31" s="57"/>
       <c r="D31" s="26"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="60"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
-      <c r="J31" s="50">
+      <c r="J31" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" s="17"/>
-      <c r="C32" s="58"/>
+      <c r="C32" s="57"/>
       <c r="D32" s="26"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="60"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
-      <c r="J32" s="50">
+      <c r="J32" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B33" s="17"/>
-      <c r="C33" s="58"/>
+      <c r="C33" s="57"/>
       <c r="D33" s="26"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="60"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
-      <c r="J33" s="50">
+      <c r="J33" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" s="17"/>
-      <c r="C34" s="58"/>
+      <c r="C34" s="57"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="60"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
-      <c r="J34" s="50">
+      <c r="J34" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B35" s="17"/>
-      <c r="C35" s="58"/>
+      <c r="C35" s="57"/>
       <c r="D35" s="26"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="60"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
-      <c r="J35" s="50">
+      <c r="J35" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="17"/>
-      <c r="C36" s="58"/>
+      <c r="C36" s="57"/>
       <c r="D36" s="26"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="60"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
-      <c r="J36" s="50">
+      <c r="J36" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="17"/>
-      <c r="C37" s="58"/>
+      <c r="C37" s="57"/>
       <c r="D37" s="26"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
-      <c r="J37" s="50">
+      <c r="J37" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B38" s="17"/>
-      <c r="C38" s="58"/>
+      <c r="C38" s="57"/>
       <c r="D38" s="26"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="60"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
-      <c r="J38" s="50">
+      <c r="J38" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="17"/>
-      <c r="C39" s="58"/>
+      <c r="C39" s="57"/>
       <c r="D39" s="26"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="60"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="59"/>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="28"/>
-      <c r="J39" s="50">
+      <c r="J39" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B40" s="17"/>
-      <c r="C40" s="58"/>
+      <c r="C40" s="57"/>
       <c r="D40" s="26"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="60"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="59"/>
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
       <c r="I40" s="28"/>
-      <c r="J40" s="50">
+      <c r="J40" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" s="17"/>
-      <c r="C41" s="58"/>
+      <c r="C41" s="57"/>
       <c r="D41" s="26"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="60"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="59"/>
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
       <c r="I41" s="28"/>
-      <c r="J41" s="50">
+      <c r="J41" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="17"/>
-      <c r="C42" s="58"/>
+      <c r="C42" s="57"/>
       <c r="D42" s="26"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="60"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="59"/>
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
       <c r="I42" s="28"/>
-      <c r="J42" s="50">
+      <c r="J42" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B43" s="17"/>
-      <c r="C43" s="58"/>
+      <c r="C43" s="57"/>
       <c r="D43" s="26"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="60"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="59"/>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
-      <c r="J43" s="50">
+      <c r="J43" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="17"/>
-      <c r="C44" s="58"/>
+      <c r="C44" s="57"/>
       <c r="D44" s="26"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="60"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="59"/>
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
       <c r="I44" s="28"/>
-      <c r="J44" s="50">
+      <c r="J44" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" s="17"/>
-      <c r="C45" s="58"/>
+      <c r="C45" s="57"/>
       <c r="D45" s="26"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="60"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="59"/>
       <c r="G45" s="28"/>
       <c r="H45" s="28"/>
       <c r="I45" s="28"/>
-      <c r="J45" s="50">
+      <c r="J45" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="17"/>
-      <c r="C46" s="58"/>
+      <c r="C46" s="57"/>
       <c r="D46" s="26"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="61"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="60"/>
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
       <c r="I46" s="28"/>
-      <c r="J46" s="50">
+      <c r="J46" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B47" s="17"/>
-      <c r="C47" s="58"/>
+      <c r="C47" s="57"/>
       <c r="D47" s="26"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="61"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="60"/>
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
       <c r="I47" s="28"/>
-      <c r="J47" s="64">
+      <c r="J47" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B48" s="17"/>
-      <c r="C48" s="58"/>
+      <c r="C48" s="57"/>
       <c r="D48" s="26"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="61"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="60"/>
       <c r="G48" s="28"/>
       <c r="H48" s="28"/>
       <c r="I48" s="28"/>
-      <c r="J48" s="50">
+      <c r="J48" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B49" s="17"/>
-      <c r="C49" s="58"/>
+      <c r="C49" s="57"/>
       <c r="D49" s="26"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="61"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="60"/>
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
-      <c r="J49" s="50">
+      <c r="J49" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B50" s="17"/>
-      <c r="C50" s="58"/>
+      <c r="C50" s="57"/>
       <c r="D50" s="26"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="61"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="60"/>
       <c r="G50" s="28"/>
       <c r="H50" s="28"/>
       <c r="I50" s="28"/>
-      <c r="J50" s="50">
+      <c r="J50" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B51" s="17"/>
-      <c r="C51" s="58"/>
+      <c r="C51" s="57"/>
       <c r="D51" s="26"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="61"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="60"/>
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
       <c r="I51" s="28"/>
-      <c r="J51" s="50">
+      <c r="J51" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B52" s="17"/>
-      <c r="C52" s="58"/>
+      <c r="C52" s="57"/>
       <c r="D52" s="26"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="61"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="60"/>
       <c r="G52" s="28"/>
       <c r="H52" s="28"/>
       <c r="I52" s="28"/>
-      <c r="J52" s="50">
+      <c r="J52" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B53" s="17"/>
-      <c r="C53" s="58"/>
+      <c r="C53" s="57"/>
       <c r="D53" s="26"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="61"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="60"/>
       <c r="G53" s="28"/>
       <c r="H53" s="28"/>
       <c r="I53" s="28"/>
-      <c r="J53" s="50">
+      <c r="J53" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B54" s="17"/>
-      <c r="C54" s="58"/>
+      <c r="C54" s="57"/>
       <c r="D54" s="26"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="61"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="60"/>
       <c r="G54" s="28"/>
       <c r="H54" s="28"/>
       <c r="I54" s="28"/>
-      <c r="J54" s="50">
+      <c r="J54" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B55" s="17"/>
-      <c r="C55" s="58"/>
+      <c r="C55" s="57"/>
       <c r="D55" s="26"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="61"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="60"/>
       <c r="G55" s="28"/>
       <c r="H55" s="28"/>
       <c r="I55" s="28"/>
-      <c r="J55" s="50">
+      <c r="J55" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B56" s="17"/>
-      <c r="C56" s="58"/>
+      <c r="C56" s="57"/>
       <c r="D56" s="26"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="61"/>
+      <c r="E56" s="57"/>
+      <c r="F56" s="60"/>
       <c r="G56" s="28"/>
       <c r="H56" s="28"/>
       <c r="I56" s="28"/>
-      <c r="J56" s="50">
+      <c r="J56" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B57" s="17"/>
-      <c r="C57" s="58"/>
+      <c r="C57" s="57"/>
       <c r="D57" s="26"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="61"/>
+      <c r="E57" s="57"/>
+      <c r="F57" s="60"/>
       <c r="G57" s="28"/>
       <c r="H57" s="28"/>
       <c r="I57" s="28"/>
-      <c r="J57" s="50">
+      <c r="J57" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B58" s="17"/>
-      <c r="C58" s="58"/>
+      <c r="C58" s="57"/>
       <c r="D58" s="26"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="61"/>
+      <c r="E58" s="57"/>
+      <c r="F58" s="60"/>
       <c r="G58" s="28"/>
       <c r="H58" s="28"/>
       <c r="I58" s="28"/>
-      <c r="J58" s="50">
+      <c r="J58" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B59" s="17"/>
-      <c r="C59" s="58"/>
+      <c r="C59" s="57"/>
       <c r="D59" s="26"/>
-      <c r="E59" s="58"/>
-      <c r="F59" s="61"/>
+      <c r="E59" s="57"/>
+      <c r="F59" s="60"/>
       <c r="G59" s="28"/>
       <c r="H59" s="28"/>
       <c r="I59" s="28"/>
-      <c r="J59" s="50">
+      <c r="J59" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B60" s="17"/>
-      <c r="C60" s="58"/>
+      <c r="C60" s="57"/>
       <c r="D60" s="26"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="61"/>
+      <c r="E60" s="57"/>
+      <c r="F60" s="60"/>
       <c r="G60" s="28"/>
       <c r="H60" s="28"/>
       <c r="I60" s="28"/>
-      <c r="J60" s="50">
+      <c r="J60" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B61" s="17"/>
-      <c r="C61" s="58"/>
+      <c r="C61" s="57"/>
       <c r="D61" s="26"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="61"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="60"/>
       <c r="G61" s="28"/>
       <c r="H61" s="28"/>
       <c r="I61" s="28"/>
-      <c r="J61" s="50">
+      <c r="J61" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B62" s="17"/>
-      <c r="C62" s="58"/>
+      <c r="C62" s="57"/>
       <c r="D62" s="26"/>
-      <c r="E62" s="58"/>
-      <c r="F62" s="61"/>
+      <c r="E62" s="57"/>
+      <c r="F62" s="60"/>
       <c r="G62" s="28"/>
       <c r="H62" s="28"/>
       <c r="I62" s="28"/>
-      <c r="J62" s="50">
+      <c r="J62" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B63" s="17"/>
-      <c r="C63" s="58"/>
+      <c r="C63" s="57"/>
       <c r="D63" s="26"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="61"/>
+      <c r="E63" s="57"/>
+      <c r="F63" s="60"/>
       <c r="G63" s="28"/>
       <c r="H63" s="28"/>
       <c r="I63" s="28"/>
-      <c r="J63" s="50">
+      <c r="J63" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B64" s="17"/>
-      <c r="C64" s="58"/>
+      <c r="C64" s="57"/>
       <c r="D64" s="26"/>
-      <c r="E64" s="58"/>
-      <c r="F64" s="61"/>
+      <c r="E64" s="57"/>
+      <c r="F64" s="60"/>
       <c r="G64" s="28"/>
       <c r="H64" s="28"/>
       <c r="I64" s="28"/>
-      <c r="J64" s="50">
+      <c r="J64" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B65" s="17"/>
-      <c r="C65" s="58"/>
+      <c r="C65" s="57"/>
       <c r="D65" s="26"/>
-      <c r="E65" s="58"/>
-      <c r="F65" s="61"/>
+      <c r="E65" s="57"/>
+      <c r="F65" s="60"/>
       <c r="G65" s="28"/>
       <c r="H65" s="28"/>
       <c r="I65" s="28"/>
-      <c r="J65" s="50">
+      <c r="J65" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B66" s="17"/>
-      <c r="C66" s="58"/>
+      <c r="C66" s="57"/>
       <c r="D66" s="26"/>
-      <c r="E66" s="58"/>
-      <c r="F66" s="61"/>
+      <c r="E66" s="57"/>
+      <c r="F66" s="60"/>
       <c r="G66" s="28"/>
       <c r="H66" s="28"/>
       <c r="I66" s="28"/>
-      <c r="J66" s="50">
+      <c r="J66" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B67" s="17"/>
-      <c r="C67" s="58"/>
+      <c r="C67" s="57"/>
       <c r="D67" s="26"/>
-      <c r="E67" s="58"/>
-      <c r="F67" s="61"/>
+      <c r="E67" s="57"/>
+      <c r="F67" s="60"/>
       <c r="G67" s="28"/>
       <c r="H67" s="28"/>
       <c r="I67" s="28"/>
-      <c r="J67" s="50">
+      <c r="J67" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B68" s="17"/>
-      <c r="C68" s="58"/>
+      <c r="C68" s="57"/>
       <c r="D68" s="26"/>
-      <c r="E68" s="58"/>
-      <c r="F68" s="61"/>
+      <c r="E68" s="57"/>
+      <c r="F68" s="60"/>
       <c r="G68" s="28"/>
       <c r="H68" s="28"/>
       <c r="I68" s="28"/>
-      <c r="J68" s="50">
+      <c r="J68" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B69" s="17"/>
-      <c r="C69" s="58"/>
+      <c r="C69" s="57"/>
       <c r="D69" s="26"/>
-      <c r="E69" s="58"/>
-      <c r="F69" s="61"/>
+      <c r="E69" s="57"/>
+      <c r="F69" s="60"/>
       <c r="G69" s="28"/>
       <c r="H69" s="28"/>
       <c r="I69" s="28"/>
-      <c r="J69" s="50">
+      <c r="J69" s="49">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B70" s="17"/>
-      <c r="C70" s="59"/>
+      <c r="C70" s="58"/>
       <c r="D70" s="26"/>
-      <c r="E70" s="59"/>
-      <c r="F70" s="62"/>
-      <c r="G70" s="63"/>
-      <c r="H70" s="63"/>
-      <c r="I70" s="63"/>
-      <c r="J70" s="64">
+      <c r="E70" s="58"/>
+      <c r="F70" s="61"/>
+      <c r="G70" s="62"/>
+      <c r="H70" s="62"/>
+      <c r="I70" s="62"/>
+      <c r="J70" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B71" s="17"/>
-      <c r="C71" s="59"/>
+      <c r="C71" s="58"/>
       <c r="D71" s="26"/>
-      <c r="E71" s="59"/>
-      <c r="F71" s="62"/>
-      <c r="G71" s="63"/>
-      <c r="H71" s="63"/>
-      <c r="I71" s="63"/>
-      <c r="J71" s="64">
+      <c r="E71" s="58"/>
+      <c r="F71" s="61"/>
+      <c r="G71" s="62"/>
+      <c r="H71" s="62"/>
+      <c r="I71" s="62"/>
+      <c r="J71" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B72" s="17"/>
-      <c r="C72" s="59"/>
+      <c r="C72" s="58"/>
       <c r="D72" s="26"/>
-      <c r="E72" s="59"/>
-      <c r="F72" s="62"/>
-      <c r="G72" s="63"/>
-      <c r="H72" s="63"/>
-      <c r="I72" s="63"/>
-      <c r="J72" s="64">
+      <c r="E72" s="58"/>
+      <c r="F72" s="61"/>
+      <c r="G72" s="62"/>
+      <c r="H72" s="62"/>
+      <c r="I72" s="62"/>
+      <c r="J72" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B73" s="17"/>
-      <c r="C73" s="59"/>
+      <c r="C73" s="58"/>
       <c r="D73" s="26"/>
-      <c r="E73" s="59"/>
-      <c r="F73" s="62"/>
-      <c r="G73" s="63"/>
-      <c r="H73" s="63"/>
-      <c r="I73" s="63"/>
-      <c r="J73" s="64">
+      <c r="E73" s="58"/>
+      <c r="F73" s="61"/>
+      <c r="G73" s="62"/>
+      <c r="H73" s="62"/>
+      <c r="I73" s="62"/>
+      <c r="J73" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B74" s="17"/>
-      <c r="C74" s="59"/>
+      <c r="C74" s="58"/>
       <c r="D74" s="26"/>
-      <c r="E74" s="59"/>
-      <c r="F74" s="62"/>
-      <c r="G74" s="63"/>
-      <c r="H74" s="63"/>
-      <c r="I74" s="63"/>
-      <c r="J74" s="64">
+      <c r="E74" s="58"/>
+      <c r="F74" s="61"/>
+      <c r="G74" s="62"/>
+      <c r="H74" s="62"/>
+      <c r="I74" s="62"/>
+      <c r="J74" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B75" s="17"/>
-      <c r="C75" s="59"/>
+      <c r="C75" s="58"/>
       <c r="D75" s="26"/>
-      <c r="E75" s="59"/>
-      <c r="F75" s="62"/>
-      <c r="G75" s="63"/>
-      <c r="H75" s="63"/>
-      <c r="I75" s="63"/>
-      <c r="J75" s="64">
+      <c r="E75" s="58"/>
+      <c r="F75" s="61"/>
+      <c r="G75" s="62"/>
+      <c r="H75" s="62"/>
+      <c r="I75" s="62"/>
+      <c r="J75" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B76" s="17"/>
-      <c r="C76" s="59"/>
+      <c r="C76" s="58"/>
       <c r="D76" s="26"/>
-      <c r="E76" s="59"/>
-      <c r="F76" s="62"/>
-      <c r="G76" s="63"/>
-      <c r="H76" s="63"/>
-      <c r="I76" s="63"/>
-      <c r="J76" s="64">
+      <c r="E76" s="58"/>
+      <c r="F76" s="61"/>
+      <c r="G76" s="62"/>
+      <c r="H76" s="62"/>
+      <c r="I76" s="62"/>
+      <c r="J76" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B77" s="17"/>
-      <c r="C77" s="59"/>
+      <c r="C77" s="58"/>
       <c r="D77" s="26"/>
-      <c r="E77" s="59"/>
-      <c r="F77" s="62"/>
-      <c r="G77" s="63"/>
-      <c r="H77" s="63"/>
-      <c r="I77" s="63"/>
-      <c r="J77" s="64">
+      <c r="E77" s="58"/>
+      <c r="F77" s="61"/>
+      <c r="G77" s="62"/>
+      <c r="H77" s="62"/>
+      <c r="I77" s="62"/>
+      <c r="J77" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B78" s="17"/>
-      <c r="C78" s="59"/>
+      <c r="C78" s="58"/>
       <c r="D78" s="26"/>
-      <c r="E78" s="59"/>
-      <c r="F78" s="62"/>
-      <c r="G78" s="63"/>
-      <c r="H78" s="63"/>
-      <c r="I78" s="63"/>
-      <c r="J78" s="64">
+      <c r="E78" s="58"/>
+      <c r="F78" s="61"/>
+      <c r="G78" s="62"/>
+      <c r="H78" s="62"/>
+      <c r="I78" s="62"/>
+      <c r="J78" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B79" s="17"/>
-      <c r="C79" s="59"/>
+      <c r="C79" s="58"/>
       <c r="D79" s="26"/>
-      <c r="E79" s="59"/>
-      <c r="F79" s="62"/>
-      <c r="G79" s="63"/>
-      <c r="H79" s="63"/>
-      <c r="I79" s="63"/>
-      <c r="J79" s="64">
+      <c r="E79" s="58"/>
+      <c r="F79" s="61"/>
+      <c r="G79" s="62"/>
+      <c r="H79" s="62"/>
+      <c r="I79" s="62"/>
+      <c r="J79" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B80" s="17"/>
-      <c r="C80" s="59"/>
+      <c r="C80" s="58"/>
       <c r="D80" s="26"/>
-      <c r="E80" s="59"/>
-      <c r="F80" s="62"/>
-      <c r="G80" s="63"/>
-      <c r="H80" s="63"/>
-      <c r="I80" s="63"/>
-      <c r="J80" s="64">
+      <c r="E80" s="58"/>
+      <c r="F80" s="61"/>
+      <c r="G80" s="62"/>
+      <c r="H80" s="62"/>
+      <c r="I80" s="62"/>
+      <c r="J80" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B81" s="17"/>
-      <c r="C81" s="59"/>
+      <c r="C81" s="58"/>
       <c r="D81" s="26"/>
-      <c r="E81" s="59"/>
-      <c r="F81" s="62"/>
-      <c r="G81" s="63"/>
-      <c r="H81" s="63"/>
-      <c r="I81" s="63"/>
-      <c r="J81" s="64">
+      <c r="E81" s="58"/>
+      <c r="F81" s="61"/>
+      <c r="G81" s="62"/>
+      <c r="H81" s="62"/>
+      <c r="I81" s="62"/>
+      <c r="J81" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B82" s="17"/>
-      <c r="C82" s="59"/>
+      <c r="C82" s="58"/>
       <c r="D82" s="26"/>
-      <c r="E82" s="59"/>
-      <c r="F82" s="62"/>
-      <c r="G82" s="63"/>
-      <c r="H82" s="63"/>
-      <c r="I82" s="63"/>
-      <c r="J82" s="64">
+      <c r="E82" s="58"/>
+      <c r="F82" s="61"/>
+      <c r="G82" s="62"/>
+      <c r="H82" s="62"/>
+      <c r="I82" s="62"/>
+      <c r="J82" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B83" s="17"/>
-      <c r="C83" s="59"/>
+      <c r="C83" s="58"/>
       <c r="D83" s="26"/>
-      <c r="E83" s="59"/>
-      <c r="F83" s="62"/>
-      <c r="G83" s="63"/>
-      <c r="H83" s="63"/>
-      <c r="I83" s="63"/>
-      <c r="J83" s="64">
+      <c r="E83" s="58"/>
+      <c r="F83" s="61"/>
+      <c r="G83" s="62"/>
+      <c r="H83" s="62"/>
+      <c r="I83" s="62"/>
+      <c r="J83" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B84" s="17"/>
-      <c r="C84" s="59"/>
+      <c r="C84" s="58"/>
       <c r="D84" s="26"/>
-      <c r="E84" s="59"/>
-      <c r="F84" s="62"/>
-      <c r="G84" s="63"/>
-      <c r="H84" s="63"/>
-      <c r="I84" s="63"/>
-      <c r="J84" s="64">
+      <c r="E84" s="58"/>
+      <c r="F84" s="61"/>
+      <c r="G84" s="62"/>
+      <c r="H84" s="62"/>
+      <c r="I84" s="62"/>
+      <c r="J84" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B85" s="17"/>
-      <c r="C85" s="59"/>
+      <c r="C85" s="58"/>
       <c r="D85" s="26"/>
-      <c r="E85" s="59"/>
-      <c r="F85" s="62"/>
-      <c r="G85" s="63"/>
-      <c r="H85" s="63"/>
-      <c r="I85" s="63"/>
-      <c r="J85" s="64">
+      <c r="E85" s="58"/>
+      <c r="F85" s="61"/>
+      <c r="G85" s="62"/>
+      <c r="H85" s="62"/>
+      <c r="I85" s="62"/>
+      <c r="J85" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B86" s="17"/>
-      <c r="C86" s="59"/>
+      <c r="C86" s="58"/>
       <c r="D86" s="26"/>
-      <c r="E86" s="59"/>
-      <c r="F86" s="62"/>
-      <c r="G86" s="63"/>
-      <c r="H86" s="63"/>
-      <c r="I86" s="63"/>
-      <c r="J86" s="64">
+      <c r="E86" s="58"/>
+      <c r="F86" s="61"/>
+      <c r="G86" s="62"/>
+      <c r="H86" s="62"/>
+      <c r="I86" s="62"/>
+      <c r="J86" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B87" s="17"/>
-      <c r="C87" s="59"/>
+      <c r="C87" s="58"/>
       <c r="D87" s="26"/>
-      <c r="E87" s="59"/>
-      <c r="F87" s="62"/>
-      <c r="G87" s="63"/>
-      <c r="H87" s="63"/>
-      <c r="I87" s="63"/>
-      <c r="J87" s="64">
+      <c r="E87" s="58"/>
+      <c r="F87" s="61"/>
+      <c r="G87" s="62"/>
+      <c r="H87" s="62"/>
+      <c r="I87" s="62"/>
+      <c r="J87" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="17"/>
-      <c r="C88" s="59"/>
+      <c r="C88" s="58"/>
       <c r="D88" s="26"/>
-      <c r="E88" s="59"/>
-      <c r="F88" s="62"/>
-      <c r="G88" s="63"/>
-      <c r="H88" s="63"/>
-      <c r="I88" s="63"/>
-      <c r="J88" s="64">
+      <c r="E88" s="58"/>
+      <c r="F88" s="61"/>
+      <c r="G88" s="62"/>
+      <c r="H88" s="62"/>
+      <c r="I88" s="62"/>
+      <c r="J88" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B89" s="17"/>
-      <c r="C89" s="59"/>
+      <c r="C89" s="58"/>
       <c r="D89" s="26"/>
-      <c r="E89" s="59"/>
-      <c r="F89" s="62"/>
-      <c r="G89" s="63"/>
-      <c r="H89" s="63"/>
-      <c r="I89" s="63"/>
-      <c r="J89" s="64">
+      <c r="E89" s="58"/>
+      <c r="F89" s="61"/>
+      <c r="G89" s="62"/>
+      <c r="H89" s="62"/>
+      <c r="I89" s="62"/>
+      <c r="J89" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B90" s="17"/>
-      <c r="C90" s="59"/>
+      <c r="C90" s="58"/>
       <c r="D90" s="26"/>
-      <c r="E90" s="59"/>
-      <c r="F90" s="62"/>
-      <c r="G90" s="63"/>
-      <c r="H90" s="63"/>
-      <c r="I90" s="63"/>
-      <c r="J90" s="64">
+      <c r="E90" s="58"/>
+      <c r="F90" s="61"/>
+      <c r="G90" s="62"/>
+      <c r="H90" s="62"/>
+      <c r="I90" s="62"/>
+      <c r="J90" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B91" s="17"/>
-      <c r="C91" s="59"/>
+      <c r="C91" s="58"/>
       <c r="D91" s="26"/>
-      <c r="E91" s="59"/>
-      <c r="F91" s="62"/>
-      <c r="G91" s="63"/>
-      <c r="H91" s="63"/>
-      <c r="I91" s="63"/>
-      <c r="J91" s="64">
+      <c r="E91" s="58"/>
+      <c r="F91" s="61"/>
+      <c r="G91" s="62"/>
+      <c r="H91" s="62"/>
+      <c r="I91" s="62"/>
+      <c r="J91" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B92" s="17"/>
-      <c r="C92" s="59"/>
+      <c r="C92" s="58"/>
       <c r="D92" s="26"/>
-      <c r="E92" s="59"/>
-      <c r="F92" s="62"/>
-      <c r="G92" s="63"/>
-      <c r="H92" s="63"/>
-      <c r="I92" s="63"/>
-      <c r="J92" s="64">
+      <c r="E92" s="58"/>
+      <c r="F92" s="61"/>
+      <c r="G92" s="62"/>
+      <c r="H92" s="62"/>
+      <c r="I92" s="62"/>
+      <c r="J92" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B93" s="17"/>
-      <c r="C93" s="59"/>
+      <c r="C93" s="58"/>
       <c r="D93" s="26"/>
-      <c r="E93" s="59"/>
-      <c r="F93" s="62"/>
-      <c r="G93" s="63"/>
-      <c r="H93" s="63"/>
-      <c r="I93" s="63"/>
-      <c r="J93" s="64">
+      <c r="E93" s="58"/>
+      <c r="F93" s="61"/>
+      <c r="G93" s="62"/>
+      <c r="H93" s="62"/>
+      <c r="I93" s="62"/>
+      <c r="J93" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B94" s="17"/>
-      <c r="C94" s="59"/>
+      <c r="C94" s="58"/>
       <c r="D94" s="26"/>
-      <c r="E94" s="59"/>
-      <c r="F94" s="62"/>
-      <c r="G94" s="63"/>
-      <c r="H94" s="63"/>
-      <c r="I94" s="63"/>
-      <c r="J94" s="64">
+      <c r="E94" s="58"/>
+      <c r="F94" s="61"/>
+      <c r="G94" s="62"/>
+      <c r="H94" s="62"/>
+      <c r="I94" s="62"/>
+      <c r="J94" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B95" s="17"/>
-      <c r="C95" s="59"/>
+      <c r="C95" s="58"/>
       <c r="D95" s="26"/>
-      <c r="E95" s="59"/>
-      <c r="F95" s="62"/>
-      <c r="G95" s="63"/>
-      <c r="H95" s="63"/>
-      <c r="I95" s="63"/>
-      <c r="J95" s="64">
+      <c r="E95" s="58"/>
+      <c r="F95" s="61"/>
+      <c r="G95" s="62"/>
+      <c r="H95" s="62"/>
+      <c r="I95" s="62"/>
+      <c r="J95" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B96" s="17"/>
-      <c r="C96" s="59"/>
+      <c r="C96" s="58"/>
       <c r="D96" s="26"/>
-      <c r="E96" s="59"/>
-      <c r="F96" s="62"/>
-      <c r="G96" s="63"/>
-      <c r="H96" s="63"/>
-      <c r="I96" s="63"/>
-      <c r="J96" s="64">
+      <c r="E96" s="58"/>
+      <c r="F96" s="61"/>
+      <c r="G96" s="62"/>
+      <c r="H96" s="62"/>
+      <c r="I96" s="62"/>
+      <c r="J96" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B97" s="17"/>
-      <c r="C97" s="59"/>
+      <c r="C97" s="58"/>
       <c r="D97" s="26"/>
-      <c r="E97" s="59"/>
-      <c r="F97" s="62"/>
-      <c r="G97" s="63"/>
-      <c r="H97" s="63"/>
-      <c r="I97" s="63"/>
-      <c r="J97" s="64">
+      <c r="E97" s="58"/>
+      <c r="F97" s="61"/>
+      <c r="G97" s="62"/>
+      <c r="H97" s="62"/>
+      <c r="I97" s="62"/>
+      <c r="J97" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B98" s="17"/>
-      <c r="C98" s="59"/>
+      <c r="C98" s="58"/>
       <c r="D98" s="26"/>
-      <c r="E98" s="59"/>
-      <c r="F98" s="62"/>
-      <c r="G98" s="63"/>
-      <c r="H98" s="63"/>
-      <c r="I98" s="63"/>
-      <c r="J98" s="64">
+      <c r="E98" s="58"/>
+      <c r="F98" s="61"/>
+      <c r="G98" s="62"/>
+      <c r="H98" s="62"/>
+      <c r="I98" s="62"/>
+      <c r="J98" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B99" s="17"/>
-      <c r="C99" s="59"/>
+      <c r="C99" s="58"/>
       <c r="D99" s="26"/>
-      <c r="E99" s="59"/>
-      <c r="F99" s="62"/>
-      <c r="G99" s="63"/>
-      <c r="H99" s="63"/>
-      <c r="I99" s="63"/>
-      <c r="J99" s="64">
+      <c r="E99" s="58"/>
+      <c r="F99" s="61"/>
+      <c r="G99" s="62"/>
+      <c r="H99" s="62"/>
+      <c r="I99" s="62"/>
+      <c r="J99" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B100" s="17"/>
-      <c r="C100" s="59"/>
+      <c r="C100" s="58"/>
       <c r="D100" s="26"/>
-      <c r="E100" s="59"/>
-      <c r="F100" s="62"/>
-      <c r="G100" s="63"/>
-      <c r="H100" s="63"/>
-      <c r="I100" s="63"/>
-      <c r="J100" s="64">
+      <c r="E100" s="58"/>
+      <c r="F100" s="61"/>
+      <c r="G100" s="62"/>
+      <c r="H100" s="62"/>
+      <c r="I100" s="62"/>
+      <c r="J100" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B101" s="17"/>
-      <c r="C101" s="59"/>
+      <c r="C101" s="58"/>
       <c r="D101" s="26"/>
-      <c r="E101" s="59"/>
-      <c r="F101" s="62"/>
-      <c r="G101" s="63"/>
-      <c r="H101" s="63"/>
-      <c r="I101" s="63"/>
-      <c r="J101" s="64">
+      <c r="E101" s="58"/>
+      <c r="F101" s="61"/>
+      <c r="G101" s="62"/>
+      <c r="H101" s="62"/>
+      <c r="I101" s="62"/>
+      <c r="J101" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B102" s="17"/>
-      <c r="C102" s="59"/>
+      <c r="C102" s="58"/>
       <c r="D102" s="26"/>
-      <c r="E102" s="59"/>
-      <c r="F102" s="62"/>
-      <c r="G102" s="63"/>
-      <c r="H102" s="63"/>
-      <c r="I102" s="63"/>
-      <c r="J102" s="64">
+      <c r="E102" s="58"/>
+      <c r="F102" s="61"/>
+      <c r="G102" s="62"/>
+      <c r="H102" s="62"/>
+      <c r="I102" s="62"/>
+      <c r="J102" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B103" s="17"/>
-      <c r="C103" s="59"/>
+      <c r="C103" s="58"/>
       <c r="D103" s="26"/>
-      <c r="E103" s="59"/>
-      <c r="F103" s="62"/>
-      <c r="G103" s="63"/>
-      <c r="H103" s="63"/>
-      <c r="I103" s="63"/>
-      <c r="J103" s="64">
+      <c r="E103" s="58"/>
+      <c r="F103" s="61"/>
+      <c r="G103" s="62"/>
+      <c r="H103" s="62"/>
+      <c r="I103" s="62"/>
+      <c r="J103" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B104" s="17"/>
-      <c r="C104" s="59"/>
+      <c r="C104" s="58"/>
       <c r="D104" s="26"/>
-      <c r="E104" s="59"/>
-      <c r="F104" s="62"/>
-      <c r="G104" s="63"/>
-      <c r="H104" s="63"/>
-      <c r="I104" s="63"/>
-      <c r="J104" s="64">
+      <c r="E104" s="58"/>
+      <c r="F104" s="61"/>
+      <c r="G104" s="62"/>
+      <c r="H104" s="62"/>
+      <c r="I104" s="62"/>
+      <c r="J104" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B105" s="17"/>
-      <c r="C105" s="59"/>
+      <c r="C105" s="58"/>
       <c r="D105" s="26"/>
-      <c r="E105" s="59"/>
-      <c r="F105" s="62"/>
-      <c r="G105" s="63"/>
-      <c r="H105" s="63"/>
-      <c r="I105" s="63"/>
-      <c r="J105" s="64">
+      <c r="E105" s="58"/>
+      <c r="F105" s="61"/>
+      <c r="G105" s="62"/>
+      <c r="H105" s="62"/>
+      <c r="I105" s="62"/>
+      <c r="J105" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B106" s="17"/>
-      <c r="C106" s="59"/>
+      <c r="C106" s="58"/>
       <c r="D106" s="26"/>
-      <c r="E106" s="59"/>
-      <c r="F106" s="62"/>
-      <c r="G106" s="63"/>
-      <c r="H106" s="63"/>
-      <c r="I106" s="63"/>
-      <c r="J106" s="64">
+      <c r="E106" s="58"/>
+      <c r="F106" s="61"/>
+      <c r="G106" s="62"/>
+      <c r="H106" s="62"/>
+      <c r="I106" s="62"/>
+      <c r="J106" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B107" s="17"/>
-      <c r="C107" s="59"/>
+      <c r="C107" s="58"/>
       <c r="D107" s="26"/>
-      <c r="E107" s="59"/>
-      <c r="F107" s="62"/>
-      <c r="G107" s="63"/>
-      <c r="H107" s="63"/>
-      <c r="I107" s="63"/>
-      <c r="J107" s="64">
+      <c r="E107" s="58"/>
+      <c r="F107" s="61"/>
+      <c r="G107" s="62"/>
+      <c r="H107" s="62"/>
+      <c r="I107" s="62"/>
+      <c r="J107" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B108" s="17"/>
-      <c r="C108" s="59"/>
+      <c r="C108" s="58"/>
       <c r="D108" s="26"/>
-      <c r="E108" s="59"/>
-      <c r="F108" s="62"/>
-      <c r="G108" s="63"/>
-      <c r="H108" s="63"/>
-      <c r="I108" s="63"/>
-      <c r="J108" s="64">
+      <c r="E108" s="58"/>
+      <c r="F108" s="61"/>
+      <c r="G108" s="62"/>
+      <c r="H108" s="62"/>
+      <c r="I108" s="62"/>
+      <c r="J108" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B109" s="17"/>
-      <c r="C109" s="59"/>
+      <c r="C109" s="58"/>
       <c r="D109" s="26"/>
-      <c r="E109" s="59"/>
-      <c r="F109" s="62"/>
-      <c r="G109" s="63"/>
-      <c r="H109" s="63"/>
-      <c r="I109" s="63"/>
-      <c r="J109" s="64">
+      <c r="E109" s="58"/>
+      <c r="F109" s="61"/>
+      <c r="G109" s="62"/>
+      <c r="H109" s="62"/>
+      <c r="I109" s="62"/>
+      <c r="J109" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B110" s="17"/>
-      <c r="C110" s="59"/>
+      <c r="C110" s="58"/>
       <c r="D110" s="26"/>
-      <c r="E110" s="59"/>
-      <c r="F110" s="62"/>
-      <c r="G110" s="63"/>
-      <c r="H110" s="63"/>
-      <c r="I110" s="63"/>
-      <c r="J110" s="64">
+      <c r="E110" s="58"/>
+      <c r="F110" s="61"/>
+      <c r="G110" s="62"/>
+      <c r="H110" s="62"/>
+      <c r="I110" s="62"/>
+      <c r="J110" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B111" s="17"/>
-      <c r="C111" s="59"/>
+      <c r="C111" s="58"/>
       <c r="D111" s="26"/>
-      <c r="E111" s="59"/>
-      <c r="F111" s="62"/>
-      <c r="G111" s="63"/>
-      <c r="H111" s="63"/>
-      <c r="I111" s="63"/>
-      <c r="J111" s="64">
+      <c r="E111" s="58"/>
+      <c r="F111" s="61"/>
+      <c r="G111" s="62"/>
+      <c r="H111" s="62"/>
+      <c r="I111" s="62"/>
+      <c r="J111" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B112" s="17"/>
-      <c r="C112" s="59"/>
+      <c r="C112" s="58"/>
       <c r="D112" s="26"/>
-      <c r="E112" s="59"/>
-      <c r="F112" s="62"/>
-      <c r="G112" s="63"/>
-      <c r="H112" s="63"/>
-      <c r="I112" s="63"/>
-      <c r="J112" s="64">
+      <c r="E112" s="58"/>
+      <c r="F112" s="61"/>
+      <c r="G112" s="62"/>
+      <c r="H112" s="62"/>
+      <c r="I112" s="62"/>
+      <c r="J112" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B113" s="17"/>
-      <c r="C113" s="59"/>
+      <c r="C113" s="58"/>
       <c r="D113" s="26"/>
-      <c r="E113" s="59"/>
-      <c r="F113" s="62"/>
-      <c r="G113" s="63"/>
-      <c r="H113" s="63"/>
-      <c r="I113" s="63"/>
-      <c r="J113" s="64">
+      <c r="E113" s="58"/>
+      <c r="F113" s="61"/>
+      <c r="G113" s="62"/>
+      <c r="H113" s="62"/>
+      <c r="I113" s="62"/>
+      <c r="J113" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B114" s="17"/>
-      <c r="C114" s="59"/>
+      <c r="C114" s="58"/>
       <c r="D114" s="26"/>
-      <c r="E114" s="59"/>
-      <c r="F114" s="62"/>
-      <c r="G114" s="63"/>
-      <c r="H114" s="63"/>
-      <c r="I114" s="63"/>
-      <c r="J114" s="64">
+      <c r="E114" s="58"/>
+      <c r="F114" s="61"/>
+      <c r="G114" s="62"/>
+      <c r="H114" s="62"/>
+      <c r="I114" s="62"/>
+      <c r="J114" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B115" s="17"/>
-      <c r="C115" s="59"/>
+      <c r="C115" s="58"/>
       <c r="D115" s="26"/>
-      <c r="E115" s="59"/>
-      <c r="F115" s="62"/>
-      <c r="G115" s="63"/>
-      <c r="H115" s="63"/>
-      <c r="I115" s="63"/>
-      <c r="J115" s="64">
+      <c r="E115" s="58"/>
+      <c r="F115" s="61"/>
+      <c r="G115" s="62"/>
+      <c r="H115" s="62"/>
+      <c r="I115" s="62"/>
+      <c r="J115" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="17"/>
-      <c r="C116" s="59"/>
+      <c r="C116" s="58"/>
       <c r="D116" s="26"/>
-      <c r="E116" s="59"/>
-      <c r="F116" s="62"/>
-      <c r="G116" s="63"/>
-      <c r="H116" s="63"/>
-      <c r="I116" s="63"/>
-      <c r="J116" s="64">
+      <c r="E116" s="58"/>
+      <c r="F116" s="61"/>
+      <c r="G116" s="62"/>
+      <c r="H116" s="62"/>
+      <c r="I116" s="62"/>
+      <c r="J116" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B117" s="17"/>
-      <c r="C117" s="59"/>
+      <c r="C117" s="58"/>
       <c r="D117" s="26"/>
-      <c r="E117" s="59"/>
-      <c r="F117" s="62"/>
-      <c r="G117" s="63"/>
-      <c r="H117" s="63"/>
-      <c r="I117" s="63"/>
-      <c r="J117" s="64">
+      <c r="E117" s="58"/>
+      <c r="F117" s="61"/>
+      <c r="G117" s="62"/>
+      <c r="H117" s="62"/>
+      <c r="I117" s="62"/>
+      <c r="J117" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B118" s="17"/>
-      <c r="C118" s="59"/>
+      <c r="C118" s="58"/>
       <c r="D118" s="26"/>
-      <c r="E118" s="59"/>
-      <c r="F118" s="62"/>
-      <c r="G118" s="63"/>
-      <c r="H118" s="63"/>
-      <c r="I118" s="63"/>
-      <c r="J118" s="64">
+      <c r="E118" s="58"/>
+      <c r="F118" s="61"/>
+      <c r="G118" s="62"/>
+      <c r="H118" s="62"/>
+      <c r="I118" s="62"/>
+      <c r="J118" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B119" s="17"/>
-      <c r="C119" s="59"/>
+      <c r="C119" s="58"/>
       <c r="D119" s="26"/>
-      <c r="E119" s="59"/>
-      <c r="F119" s="62"/>
-      <c r="G119" s="63"/>
-      <c r="H119" s="63"/>
-      <c r="I119" s="63"/>
-      <c r="J119" s="64">
+      <c r="E119" s="58"/>
+      <c r="F119" s="61"/>
+      <c r="G119" s="62"/>
+      <c r="H119" s="62"/>
+      <c r="I119" s="62"/>
+      <c r="J119" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B120" s="17"/>
-      <c r="C120" s="59"/>
+      <c r="C120" s="58"/>
       <c r="D120" s="26"/>
-      <c r="E120" s="59"/>
-      <c r="F120" s="62"/>
-      <c r="G120" s="63"/>
-      <c r="H120" s="63"/>
-      <c r="I120" s="63"/>
-      <c r="J120" s="64">
+      <c r="E120" s="58"/>
+      <c r="F120" s="61"/>
+      <c r="G120" s="62"/>
+      <c r="H120" s="62"/>
+      <c r="I120" s="62"/>
+      <c r="J120" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B121" s="17"/>
-      <c r="C121" s="59"/>
+      <c r="C121" s="58"/>
       <c r="D121" s="26"/>
-      <c r="E121" s="59"/>
-      <c r="F121" s="62"/>
-      <c r="G121" s="63"/>
-      <c r="H121" s="63"/>
-      <c r="I121" s="63"/>
-      <c r="J121" s="64">
+      <c r="E121" s="58"/>
+      <c r="F121" s="61"/>
+      <c r="G121" s="62"/>
+      <c r="H121" s="62"/>
+      <c r="I121" s="62"/>
+      <c r="J121" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B122" s="17"/>
-      <c r="C122" s="59"/>
+      <c r="C122" s="58"/>
       <c r="D122" s="26"/>
-      <c r="E122" s="59"/>
-      <c r="F122" s="62"/>
-      <c r="G122" s="63"/>
-      <c r="H122" s="63"/>
-      <c r="I122" s="63"/>
-      <c r="J122" s="64">
+      <c r="E122" s="58"/>
+      <c r="F122" s="61"/>
+      <c r="G122" s="62"/>
+      <c r="H122" s="62"/>
+      <c r="I122" s="62"/>
+      <c r="J122" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B123" s="17"/>
-      <c r="C123" s="59"/>
+      <c r="C123" s="58"/>
       <c r="D123" s="26"/>
-      <c r="E123" s="59"/>
-      <c r="F123" s="62"/>
-      <c r="G123" s="63"/>
-      <c r="H123" s="63"/>
-      <c r="I123" s="63"/>
-      <c r="J123" s="64">
+      <c r="E123" s="58"/>
+      <c r="F123" s="61"/>
+      <c r="G123" s="62"/>
+      <c r="H123" s="62"/>
+      <c r="I123" s="62"/>
+      <c r="J123" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B124" s="17"/>
-      <c r="C124" s="59"/>
+      <c r="C124" s="58"/>
       <c r="D124" s="26"/>
-      <c r="E124" s="59"/>
-      <c r="F124" s="62"/>
-      <c r="G124" s="63"/>
-      <c r="H124" s="63"/>
-      <c r="I124" s="63"/>
-      <c r="J124" s="64">
+      <c r="E124" s="58"/>
+      <c r="F124" s="61"/>
+      <c r="G124" s="62"/>
+      <c r="H124" s="62"/>
+      <c r="I124" s="62"/>
+      <c r="J124" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B125" s="17"/>
-      <c r="C125" s="59"/>
+      <c r="C125" s="58"/>
       <c r="D125" s="26"/>
-      <c r="E125" s="59"/>
-      <c r="F125" s="62"/>
-      <c r="G125" s="63"/>
-      <c r="H125" s="63"/>
-      <c r="I125" s="63"/>
-      <c r="J125" s="64">
+      <c r="E125" s="58"/>
+      <c r="F125" s="61"/>
+      <c r="G125" s="62"/>
+      <c r="H125" s="62"/>
+      <c r="I125" s="62"/>
+      <c r="J125" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B126" s="17"/>
-      <c r="C126" s="59"/>
+      <c r="C126" s="58"/>
       <c r="D126" s="26"/>
-      <c r="E126" s="59"/>
-      <c r="F126" s="62"/>
-      <c r="G126" s="63"/>
-      <c r="H126" s="63"/>
-      <c r="I126" s="63"/>
-      <c r="J126" s="64">
+      <c r="E126" s="58"/>
+      <c r="F126" s="61"/>
+      <c r="G126" s="62"/>
+      <c r="H126" s="62"/>
+      <c r="I126" s="62"/>
+      <c r="J126" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B127" s="17"/>
-      <c r="C127" s="59"/>
+      <c r="C127" s="58"/>
       <c r="D127" s="26"/>
-      <c r="E127" s="59"/>
-      <c r="F127" s="62"/>
-      <c r="G127" s="63"/>
-      <c r="H127" s="63"/>
-      <c r="I127" s="63"/>
-      <c r="J127" s="64">
+      <c r="E127" s="58"/>
+      <c r="F127" s="61"/>
+      <c r="G127" s="62"/>
+      <c r="H127" s="62"/>
+      <c r="I127" s="62"/>
+      <c r="J127" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B128" s="17"/>
-      <c r="C128" s="59"/>
+      <c r="C128" s="58"/>
       <c r="D128" s="26"/>
-      <c r="E128" s="59"/>
-      <c r="F128" s="62"/>
-      <c r="G128" s="63"/>
-      <c r="H128" s="63"/>
-      <c r="I128" s="63"/>
-      <c r="J128" s="64">
+      <c r="E128" s="58"/>
+      <c r="F128" s="61"/>
+      <c r="G128" s="62"/>
+      <c r="H128" s="62"/>
+      <c r="I128" s="62"/>
+      <c r="J128" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B129" s="17"/>
-      <c r="C129" s="59"/>
+      <c r="C129" s="58"/>
       <c r="D129" s="26"/>
-      <c r="E129" s="59"/>
-      <c r="F129" s="62"/>
-      <c r="G129" s="63"/>
-      <c r="H129" s="63"/>
-      <c r="I129" s="63"/>
-      <c r="J129" s="64">
+      <c r="E129" s="58"/>
+      <c r="F129" s="61"/>
+      <c r="G129" s="62"/>
+      <c r="H129" s="62"/>
+      <c r="I129" s="62"/>
+      <c r="J129" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B130" s="17"/>
-      <c r="C130" s="59"/>
+      <c r="C130" s="58"/>
       <c r="D130" s="26"/>
-      <c r="E130" s="59"/>
-      <c r="F130" s="62"/>
-      <c r="G130" s="63"/>
-      <c r="H130" s="63"/>
-      <c r="I130" s="63"/>
-      <c r="J130" s="64">
+      <c r="E130" s="58"/>
+      <c r="F130" s="61"/>
+      <c r="G130" s="62"/>
+      <c r="H130" s="62"/>
+      <c r="I130" s="62"/>
+      <c r="J130" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="17"/>
-      <c r="C131" s="59"/>
+      <c r="C131" s="58"/>
       <c r="D131" s="26"/>
-      <c r="E131" s="59"/>
-      <c r="F131" s="62"/>
-      <c r="G131" s="63"/>
-      <c r="H131" s="63"/>
-      <c r="I131" s="63"/>
-      <c r="J131" s="64">
+      <c r="E131" s="58"/>
+      <c r="F131" s="61"/>
+      <c r="G131" s="62"/>
+      <c r="H131" s="62"/>
+      <c r="I131" s="62"/>
+      <c r="J131" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B132" s="17"/>
-      <c r="C132" s="59"/>
+      <c r="C132" s="58"/>
       <c r="D132" s="26"/>
-      <c r="E132" s="59"/>
-      <c r="F132" s="62"/>
-      <c r="G132" s="63"/>
-      <c r="H132" s="63"/>
-      <c r="I132" s="63"/>
-      <c r="J132" s="64">
+      <c r="E132" s="58"/>
+      <c r="F132" s="61"/>
+      <c r="G132" s="62"/>
+      <c r="H132" s="62"/>
+      <c r="I132" s="62"/>
+      <c r="J132" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B133" s="17"/>
-      <c r="C133" s="59"/>
+      <c r="C133" s="58"/>
       <c r="D133" s="26"/>
-      <c r="E133" s="59"/>
-      <c r="F133" s="62"/>
-      <c r="G133" s="63"/>
-      <c r="H133" s="63"/>
-      <c r="I133" s="63"/>
-      <c r="J133" s="64">
+      <c r="E133" s="58"/>
+      <c r="F133" s="61"/>
+      <c r="G133" s="62"/>
+      <c r="H133" s="62"/>
+      <c r="I133" s="62"/>
+      <c r="J133" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B134" s="17"/>
-      <c r="C134" s="59"/>
+      <c r="C134" s="58"/>
       <c r="D134" s="26"/>
-      <c r="E134" s="59"/>
-      <c r="F134" s="62"/>
-      <c r="G134" s="63"/>
-      <c r="H134" s="63"/>
-      <c r="I134" s="63"/>
-      <c r="J134" s="64">
+      <c r="E134" s="58"/>
+      <c r="F134" s="61"/>
+      <c r="G134" s="62"/>
+      <c r="H134" s="62"/>
+      <c r="I134" s="62"/>
+      <c r="J134" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B135" s="17"/>
-      <c r="C135" s="59"/>
+      <c r="C135" s="58"/>
       <c r="D135" s="26"/>
-      <c r="E135" s="59"/>
-      <c r="F135" s="62"/>
-      <c r="G135" s="63"/>
-      <c r="H135" s="63"/>
-      <c r="I135" s="63"/>
-      <c r="J135" s="64">
+      <c r="E135" s="58"/>
+      <c r="F135" s="61"/>
+      <c r="G135" s="62"/>
+      <c r="H135" s="62"/>
+      <c r="I135" s="62"/>
+      <c r="J135" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B136" s="17"/>
-      <c r="C136" s="59"/>
+      <c r="C136" s="58"/>
       <c r="D136" s="26"/>
-      <c r="E136" s="59"/>
-      <c r="F136" s="62"/>
-      <c r="G136" s="63"/>
-      <c r="H136" s="63"/>
-      <c r="I136" s="63"/>
-      <c r="J136" s="64">
+      <c r="E136" s="58"/>
+      <c r="F136" s="61"/>
+      <c r="G136" s="62"/>
+      <c r="H136" s="62"/>
+      <c r="I136" s="62"/>
+      <c r="J136" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B137" s="17"/>
-      <c r="C137" s="59"/>
+      <c r="C137" s="58"/>
       <c r="D137" s="26"/>
-      <c r="E137" s="59"/>
-      <c r="F137" s="62"/>
-      <c r="G137" s="63"/>
-      <c r="H137" s="63"/>
-      <c r="I137" s="63"/>
-      <c r="J137" s="64">
+      <c r="E137" s="58"/>
+      <c r="F137" s="61"/>
+      <c r="G137" s="62"/>
+      <c r="H137" s="62"/>
+      <c r="I137" s="62"/>
+      <c r="J137" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B138" s="17"/>
-      <c r="C138" s="59"/>
+      <c r="C138" s="58"/>
       <c r="D138" s="26"/>
-      <c r="E138" s="59"/>
-      <c r="F138" s="62"/>
-      <c r="G138" s="63"/>
-      <c r="H138" s="63"/>
-      <c r="I138" s="63"/>
-      <c r="J138" s="64">
+      <c r="E138" s="58"/>
+      <c r="F138" s="61"/>
+      <c r="G138" s="62"/>
+      <c r="H138" s="62"/>
+      <c r="I138" s="62"/>
+      <c r="J138" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B139" s="17"/>
-      <c r="C139" s="59"/>
+      <c r="C139" s="58"/>
       <c r="D139" s="26"/>
-      <c r="E139" s="59"/>
-      <c r="F139" s="62"/>
-      <c r="G139" s="63"/>
-      <c r="H139" s="63"/>
-      <c r="I139" s="63"/>
-      <c r="J139" s="64">
+      <c r="E139" s="58"/>
+      <c r="F139" s="61"/>
+      <c r="G139" s="62"/>
+      <c r="H139" s="62"/>
+      <c r="I139" s="62"/>
+      <c r="J139" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B140" s="17"/>
-      <c r="C140" s="59"/>
+      <c r="C140" s="58"/>
       <c r="D140" s="26"/>
-      <c r="E140" s="59"/>
-      <c r="F140" s="62"/>
-      <c r="G140" s="63"/>
-      <c r="H140" s="63"/>
-      <c r="I140" s="63"/>
-      <c r="J140" s="64">
+      <c r="E140" s="58"/>
+      <c r="F140" s="61"/>
+      <c r="G140" s="62"/>
+      <c r="H140" s="62"/>
+      <c r="I140" s="62"/>
+      <c r="J140" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B141" s="17"/>
-      <c r="C141" s="59"/>
+      <c r="C141" s="58"/>
       <c r="D141" s="26"/>
-      <c r="E141" s="59"/>
-      <c r="F141" s="62"/>
-      <c r="G141" s="63"/>
-      <c r="H141" s="63"/>
-      <c r="I141" s="63"/>
-      <c r="J141" s="64">
+      <c r="E141" s="58"/>
+      <c r="F141" s="61"/>
+      <c r="G141" s="62"/>
+      <c r="H141" s="62"/>
+      <c r="I141" s="62"/>
+      <c r="J141" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B142" s="17"/>
-      <c r="C142" s="59"/>
+      <c r="C142" s="58"/>
       <c r="D142" s="26"/>
-      <c r="E142" s="59"/>
-      <c r="F142" s="62"/>
-      <c r="G142" s="63"/>
-      <c r="H142" s="63"/>
-      <c r="I142" s="63"/>
-      <c r="J142" s="64">
+      <c r="E142" s="58"/>
+      <c r="F142" s="61"/>
+      <c r="G142" s="62"/>
+      <c r="H142" s="62"/>
+      <c r="I142" s="62"/>
+      <c r="J142" s="63">
         <f>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="17"/>
-      <c r="C143" s="66"/>
+      <c r="C143" s="65"/>
       <c r="D143" s="26"/>
-      <c r="E143" s="66"/>
-      <c r="F143" s="67"/>
-      <c r="G143" s="63"/>
-      <c r="H143" s="63"/>
-      <c r="I143" s="63"/>
-      <c r="J143" s="64"/>
+      <c r="E143" s="65"/>
+      <c r="F143" s="66"/>
+      <c r="G143" s="62"/>
+      <c r="H143" s="62"/>
+      <c r="I143" s="62"/>
+      <c r="J143" s="63"/>
     </row>
     <row r="144" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B144" s="17"/>
-      <c r="C144" s="66"/>
+      <c r="C144" s="65"/>
       <c r="D144" s="26"/>
-      <c r="E144" s="66"/>
-      <c r="F144" s="67"/>
-      <c r="G144" s="63"/>
-      <c r="H144" s="63"/>
-      <c r="I144" s="63"/>
-      <c r="J144" s="64"/>
+      <c r="E144" s="65"/>
+      <c r="F144" s="66"/>
+      <c r="G144" s="62"/>
+      <c r="H144" s="62"/>
+      <c r="I144" s="62"/>
+      <c r="J144" s="63"/>
     </row>
     <row r="145" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B145" s="17"/>
-      <c r="C145" s="66"/>
+      <c r="C145" s="65"/>
       <c r="D145" s="26"/>
-      <c r="E145" s="66"/>
-      <c r="F145" s="67"/>
-      <c r="G145" s="63"/>
-      <c r="H145" s="63"/>
-      <c r="I145" s="63"/>
-      <c r="J145" s="64"/>
+      <c r="E145" s="65"/>
+      <c r="F145" s="66"/>
+      <c r="G145" s="62"/>
+      <c r="H145" s="62"/>
+      <c r="I145" s="62"/>
+      <c r="J145" s="63"/>
     </row>
     <row r="146" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B146" s="17"/>
-      <c r="C146" s="66"/>
+      <c r="C146" s="65"/>
       <c r="D146" s="26"/>
-      <c r="E146" s="66"/>
-      <c r="F146" s="67"/>
-      <c r="G146" s="63"/>
-      <c r="H146" s="63"/>
-      <c r="I146" s="63"/>
-      <c r="J146" s="64"/>
+      <c r="E146" s="65"/>
+      <c r="F146" s="66"/>
+      <c r="G146" s="62"/>
+      <c r="H146" s="62"/>
+      <c r="I146" s="62"/>
+      <c r="J146" s="63"/>
     </row>
     <row r="147" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B147" s="17"/>
-      <c r="C147" s="66"/>
+      <c r="C147" s="65"/>
       <c r="D147" s="26"/>
-      <c r="E147" s="66"/>
-      <c r="F147" s="67"/>
-      <c r="G147" s="63"/>
-      <c r="H147" s="63"/>
-      <c r="I147" s="63"/>
-      <c r="J147" s="64"/>
+      <c r="E147" s="65"/>
+      <c r="F147" s="66"/>
+      <c r="G147" s="62"/>
+      <c r="H147" s="62"/>
+      <c r="I147" s="62"/>
+      <c r="J147" s="63"/>
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B148" s="17"/>
-      <c r="C148" s="66"/>
+      <c r="C148" s="65"/>
       <c r="D148" s="26"/>
-      <c r="E148" s="66"/>
-      <c r="F148" s="67"/>
-      <c r="G148" s="63"/>
-      <c r="H148" s="63"/>
-      <c r="I148" s="63"/>
-      <c r="J148" s="64"/>
+      <c r="E148" s="65"/>
+      <c r="F148" s="66"/>
+      <c r="G148" s="62"/>
+      <c r="H148" s="62"/>
+      <c r="I148" s="62"/>
+      <c r="J148" s="63"/>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B149" s="17"/>
-      <c r="C149" s="66"/>
+      <c r="C149" s="65"/>
       <c r="D149" s="26"/>
-      <c r="E149" s="66"/>
-      <c r="F149" s="67"/>
-      <c r="G149" s="63"/>
-      <c r="H149" s="63"/>
-      <c r="I149" s="63"/>
-      <c r="J149" s="64"/>
+      <c r="E149" s="65"/>
+      <c r="F149" s="66"/>
+      <c r="G149" s="62"/>
+      <c r="H149" s="62"/>
+      <c r="I149" s="62"/>
+      <c r="J149" s="63"/>
     </row>
     <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B150" s="17"/>
-      <c r="C150" s="66"/>
+      <c r="C150" s="65"/>
       <c r="D150" s="26"/>
-      <c r="E150" s="66"/>
-      <c r="F150" s="67"/>
-      <c r="G150" s="63"/>
-      <c r="H150" s="63"/>
-      <c r="I150" s="63"/>
-      <c r="J150" s="64"/>
+      <c r="E150" s="65"/>
+      <c r="F150" s="66"/>
+      <c r="G150" s="62"/>
+      <c r="H150" s="62"/>
+      <c r="I150" s="62"/>
+      <c r="J150" s="63"/>
     </row>
     <row r="151" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B151" s="17"/>
-      <c r="C151" s="66"/>
-      <c r="D151" s="68"/>
-      <c r="E151" s="66"/>
-      <c r="F151" s="67"/>
-      <c r="G151" s="63"/>
-      <c r="H151" s="63"/>
-      <c r="I151" s="63"/>
-      <c r="J151" s="64"/>
+      <c r="C151" s="65"/>
+      <c r="D151" s="67"/>
+      <c r="E151" s="65"/>
+      <c r="F151" s="66"/>
+      <c r="G151" s="62"/>
+      <c r="H151" s="62"/>
+      <c r="I151" s="62"/>
+      <c r="J151" s="63"/>
     </row>
     <row r="152" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B152" s="17"/>
-      <c r="C152" s="66"/>
-      <c r="D152" s="68"/>
-      <c r="E152" s="66"/>
-      <c r="F152" s="67"/>
-      <c r="G152" s="63"/>
-      <c r="H152" s="63"/>
-      <c r="I152" s="63"/>
-      <c r="J152" s="64"/>
+      <c r="C152" s="65"/>
+      <c r="D152" s="67"/>
+      <c r="E152" s="65"/>
+      <c r="F152" s="66"/>
+      <c r="G152" s="62"/>
+      <c r="H152" s="62"/>
+      <c r="I152" s="62"/>
+      <c r="J152" s="63"/>
     </row>
     <row r="153" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B153" s="17"/>
-      <c r="C153" s="66"/>
-      <c r="D153" s="68"/>
-      <c r="E153" s="66"/>
-      <c r="F153" s="67"/>
-      <c r="G153" s="63"/>
-      <c r="H153" s="63"/>
-      <c r="I153" s="63"/>
-      <c r="J153" s="64"/>
+      <c r="C153" s="65"/>
+      <c r="D153" s="67"/>
+      <c r="E153" s="65"/>
+      <c r="F153" s="66"/>
+      <c r="G153" s="62"/>
+      <c r="H153" s="62"/>
+      <c r="I153" s="62"/>
+      <c r="J153" s="63"/>
     </row>
     <row r="154" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B154" s="17"/>
-      <c r="C154" s="66"/>
-      <c r="D154" s="68"/>
-      <c r="E154" s="66"/>
-      <c r="F154" s="67"/>
-      <c r="G154" s="63"/>
-      <c r="H154" s="63"/>
-      <c r="I154" s="63"/>
-      <c r="J154" s="64"/>
+      <c r="C154" s="65"/>
+      <c r="D154" s="67"/>
+      <c r="E154" s="65"/>
+      <c r="F154" s="66"/>
+      <c r="G154" s="62"/>
+      <c r="H154" s="62"/>
+      <c r="I154" s="62"/>
+      <c r="J154" s="63"/>
     </row>
     <row r="155" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B155" s="17"/>
-      <c r="C155" s="66"/>
-      <c r="D155" s="68"/>
-      <c r="E155" s="66"/>
-      <c r="F155" s="67"/>
-      <c r="G155" s="63"/>
-      <c r="H155" s="63"/>
-      <c r="I155" s="63"/>
-      <c r="J155" s="64"/>
+      <c r="C155" s="65"/>
+      <c r="D155" s="67"/>
+      <c r="E155" s="65"/>
+      <c r="F155" s="66"/>
+      <c r="G155" s="62"/>
+      <c r="H155" s="62"/>
+      <c r="I155" s="62"/>
+      <c r="J155" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -6770,10 +6736,10 @@
     </row>
     <row r="26" spans="2:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="69"/>
+      <c r="B28" s="68"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="69"/>
+      <c r="B29" s="68"/>
       <c r="O29" t="str">
         <f>IFERROR(INDEX(Issues[Location],MATCH(0,COUNTIF(#REF!,Issues[Location]),0)),"")</f>
         <v/>
@@ -6940,572 +6906,572 @@
       <c r="S5" s="85"/>
     </row>
     <row r="6" spans="2:19" ht="204.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="51" t="s">
+      <c r="H6" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="I6" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="52" t="s">
+      <c r="K6" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="51" t="s">
+      <c r="L6" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="55" t="s">
+      <c r="M6" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="51" t="s">
+      <c r="N6" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="52" t="s">
+      <c r="O6" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="57" t="s">
+      <c r="P6" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="Q6" s="56" t="s">
+      <c r="Q6" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="51" t="s">
+      <c r="R6" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="52" t="s">
+      <c r="S6" s="51" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:19" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="51" t="s">
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="52"/>
-      <c r="L7" s="51" t="s">
+      <c r="K7" s="51"/>
+      <c r="L7" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="52" t="s">
+      <c r="M7" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="51" t="s">
+      <c r="N7" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="52" t="s">
+      <c r="O7" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="P7" s="57" t="s">
+      <c r="P7" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" s="56" t="s">
+      <c r="Q7" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="R7" s="51" t="s">
+      <c r="R7" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="52" t="s">
+      <c r="S7" s="51" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="51" t="s">
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="51"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="51" t="s">
+      <c r="H8" s="50"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="M8" s="52" t="s">
+      <c r="M8" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="N8" s="51"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="57" t="s">
+      <c r="N8" s="50"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="Q8" s="56" t="s">
+      <c r="Q8" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="R8" s="51" t="s">
+      <c r="R8" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="S8" s="52" t="s">
+      <c r="S8" s="51" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="51" t="s">
+      <c r="C9" s="52"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="M9" s="52" t="s">
+      <c r="M9" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="51"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="57" t="s">
+      <c r="N9" s="50"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="51" t="s">
+      <c r="Q9" s="55"/>
+      <c r="R9" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="S9" s="52" t="s">
+      <c r="S9" s="51" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="51" t="s">
+      <c r="C10" s="52"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="M10" s="52" t="s">
+      <c r="M10" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="N10" s="51"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="51" t="s">
+      <c r="N10" s="50"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="S10" s="52" t="s">
+      <c r="S10" s="51" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="51"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="51"/>
-      <c r="S11" s="52"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="55"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="51"/>
     </row>
     <row r="12" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="51"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="52"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="55"/>
+      <c r="Q12" s="55"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="51"/>
     </row>
     <row r="13" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="51"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="52"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="55"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="51"/>
     </row>
     <row r="14" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="52"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="55"/>
+      <c r="Q14" s="55"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="51"/>
     </row>
     <row r="15" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="51"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="52"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="51"/>
     </row>
     <row r="16" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="51"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="52"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="52"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="51"/>
     </row>
     <row r="17" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="51"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="52"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="52"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="51"/>
     </row>
     <row r="18" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="51"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="52"/>
-      <c r="P18" s="56"/>
-      <c r="Q18" s="56"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="52"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="50"/>
+      <c r="S18" s="51"/>
     </row>
     <row r="19" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="51"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="52"/>
-      <c r="P19" s="56"/>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="52"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="50"/>
+      <c r="S19" s="51"/>
     </row>
     <row r="20" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="51"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="52"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="51"/>
-      <c r="S20" s="52"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="50"/>
+      <c r="S20" s="51"/>
     </row>
     <row r="21" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="51"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="52"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="51"/>
-      <c r="S21" s="52"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="51"/>
     </row>
     <row r="22" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="51"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="52"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="51"/>
-      <c r="S22" s="52"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="51"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="50"/>
+      <c r="S22" s="51"/>
     </row>
     <row r="23" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="51"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="51"/>
-      <c r="S23" s="52"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="51"/>
     </row>
     <row r="24" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="51"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="56"/>
-      <c r="Q24" s="56"/>
-      <c r="R24" s="51"/>
-      <c r="S24" s="52"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="50"/>
+      <c r="S24" s="51"/>
     </row>
     <row r="25" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="51"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="52"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="51"/>
-      <c r="S25" s="52"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="55"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="51"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="51"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="52"/>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="56"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="52"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="51"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="50"/>
+      <c r="S26" s="51"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="51"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="52"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="51"/>
-      <c r="S27" s="52"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="51"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="55"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="51"/>
     </row>
     <row r="28" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="51"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="52"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -7716,10 +7682,10 @@
       </c>
       <c r="F3" s="91"/>
       <c r="G3" s="91"/>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="46" t="s">
         <v>105</v>
       </c>
     </row>
@@ -7737,10 +7703,10 @@
       <c r="G4" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="48">
+      <c r="I4" s="47">
         <v>1</v>
       </c>
-      <c r="K4" s="48" t="s">
+      <c r="K4" s="47" t="s">
         <v>110</v>
       </c>
     </row>
@@ -7758,10 +7724,10 @@
       <c r="G5" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="I5" s="48">
+      <c r="I5" s="47">
         <v>3</v>
       </c>
-      <c r="K5" s="48" t="s">
+      <c r="K5" s="47" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7779,10 +7745,10 @@
       <c r="G6" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="I6" s="48">
+      <c r="I6" s="47">
         <v>5</v>
       </c>
-      <c r="K6" s="48" t="s">
+      <c r="K6" s="47" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>